<commit_message>
divided event component into SportsList
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\varun\websites\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353BE49D-284D-4944-954A-ABAC6070C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B586FC-6568-460A-83DD-7B7E93AF35B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>https://wallpaperdig.com/wp-content/uploads/2021/02/XDCFVBGNHJM.jpg</t>
   </si>
   <si>
-    <t>TEnrolled</t>
-  </si>
-  <si>
     <t>https://cdn.wallpapersafari.com/3/7/SFe72B.jpg</t>
   </si>
   <si>
@@ -70,6 +67,30 @@
   </si>
   <si>
     <t>2023-10-17T11:25:00</t>
+  </si>
+  <si>
+    <t>Chess</t>
+  </si>
+  <si>
+    <t>Valorant</t>
+  </si>
+  <si>
+    <t>BGMI</t>
+  </si>
+  <si>
+    <t>Carrom</t>
+  </si>
+  <si>
+    <t>TAG</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
@@ -411,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -451,7 +472,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -462,10 +483,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -476,8 +497,8 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>21</v>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -488,11 +509,11 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
@@ -502,8 +523,8 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
-        <v>22</v>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -517,24 +538,136 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{80D4283D-615C-4D83-A5A3-985698264829}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{0085C6EE-C0F5-49CA-9EE2-CF227EDBBB6C}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{C8E7302E-CD9C-4DC3-B58E-48F4523F7726}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
event and sports image added
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\varun\websites\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B586FC-6568-460A-83DD-7B7E93AF35B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC13D58-BC61-4A1B-AB67-11CFE7221D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -57,15 +57,6 @@
     <t>Cricket</t>
   </si>
   <si>
-    <t>https://wallpaperdig.com/wp-content/uploads/2021/02/XDCFVBGNHJM.jpg</t>
-  </si>
-  <si>
-    <t>https://cdn.wallpapersafari.com/3/7/SFe72B.jpg</t>
-  </si>
-  <si>
-    <t>https://hdqwalls.com/wallpapers/basketball-hd.jpg</t>
-  </si>
-  <si>
     <t>2023-10-17T11:25:00</t>
   </si>
   <si>
@@ -91,6 +82,27 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1163848747504124019/1163871657656594562/Cricket-01.png?ex=654126f2&amp;is=652eb1f2&amp;hm=7164052bcc4ecfb45a1afd57927b6e565249872b1c36cf8c08b33ed324a41aa2&amp;=&amp;width=606&amp;height=662</t>
+  </si>
+  <si>
+    <t>Volleyball</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1163848747504124019/1163871658084405338/Volleyball.png?ex=654126f2&amp;is=652eb1f2&amp;hm=a380084f1cb56b3696d8643b5deb5986eace96e712788614119e170caf7e123f&amp;=&amp;width=606&amp;height=662</t>
+  </si>
+  <si>
+    <t>Batminton</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1163848747504124019/1163871658445119488/Badminton-01.png?ex=654126f3&amp;is=652eb1f3&amp;hm=471c57b99bcdc60f411862bdf7a01a72074a66f0d0d779b682b0c1e2c928ac67&amp;=&amp;width=606&amp;height=662</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1163848747504124019/1163871658952634428/Basketball-01.png?ex=654126f3&amp;is=652eb1f3&amp;hm=f539824e1aa7b08961f5c9f6ec608da006161916fe2176550e3401beacab893c&amp;=&amp;width=606&amp;height=662</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1163848747504124019/1163871659376251053/Chess-01.png?ex=654126f3&amp;is=652eb1f3&amp;hm=1c59ff862c2829ec507d82a8cf7d47321d2fea3cee9c20e06c983beb771688c8&amp;=&amp;width=606&amp;height=662</t>
   </si>
 </sst>
 </file>
@@ -144,11 +156,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -435,14 +450,14 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.44140625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -472,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -482,11 +497,11 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -498,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -509,10 +524,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -524,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -534,11 +549,11 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -550,21 +565,21 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -576,21 +591,21 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -602,72 +617,117 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{80D4283D-615C-4D83-A5A3-985698264829}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{0085C6EE-C0F5-49CA-9EE2-CF227EDBBB6C}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{C8E7302E-CD9C-4DC3-B58E-48F4523F7726}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{10A4F5BB-A0C6-4758-BB19-BABAA9FE455D}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{8245749E-3676-4614-AB51-65B15D0F7E41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed dark theme custom and image import format
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\varun\websites\gehusports\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC13D58-BC61-4A1B-AB67-11CFE7221D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE83A29C-15F0-4F53-8CDD-767007C9CEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Cricket</t>
   </si>
   <si>
-    <t>2023-10-17T11:25:00</t>
-  </si>
-  <si>
     <t>Chess</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>https://media.discordapp.net/attachments/1163848747504124019/1163871659376251053/Chess-01.png?ex=654126f3&amp;is=652eb1f3&amp;hm=1c59ff862c2829ec507d82a8cf7d47321d2fea3cee9c20e06c983beb771688c8&amp;=&amp;width=606&amp;height=662</t>
+  </si>
+  <si>
+    <t>2023-11-01T11:25:00</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -498,10 +498,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -524,10 +524,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -550,10 +550,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -565,21 +565,21 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -591,21 +591,21 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -617,21 +617,21 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -643,21 +643,21 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -669,21 +669,21 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -695,21 +695,21 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated for the final time
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47756F17-8884-4DC8-B7DB-18168B276052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA688ED-20AE-4977-A4E3-A5FFE17CF7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>26</v>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
formated style sheet and excel sheet along with function
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98D725F-E1A3-4456-90D7-BE923C095035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79654A86-C237-4538-9043-739BCCF32B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>2023-11-05T00:00:00</t>
+  </si>
+  <si>
+    <t>2023-11-06T00:00:00</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -558,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Add registration form for Arm Wrestling and rules section links, update event dates
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79654A86-C237-4538-9043-739BCCF32B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2ECFB-9781-411A-96AF-6D88EC6224ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>2023-11-06T00:00:00</t>
+  </si>
+  <si>
+    <t>Edate</t>
+  </si>
+  <si>
+    <t>2023-11-08T00:00:00</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -464,15 +470,15 @@
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,23 +489,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,24 +518,27 @@
       <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -536,24 +548,27 @@
       <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -563,24 +578,27 @@
       <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -590,24 +608,27 @@
       <c r="C5" s="5">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -617,24 +638,27 @@
       <c r="C6" s="5">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -644,24 +668,27 @@
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -671,22 +698,25 @@
       <c r="C8" s="5">
         <v>0</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update event end dates in JSON file.
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2ECFB-9781-411A-96AF-6D88EC6224ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB1A84-0871-4AE6-AB30-E161886D4D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>Edate</t>
   </si>
   <si>
-    <t>2023-11-08T00:00:00</t>
+    <t>2023-11-08T24:00:00</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Update event statuses in JSON file
</commit_message>
<xml_diff>
--- a/data/excel/events.xlsx
+++ b/data/excel/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB1A84-0871-4AE6-AB30-E161886D4D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29B1060-BBA6-4564-AEA7-5C731A9C364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Arm Wrestling</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>https://media.discordapp.net/attachments/1162451241872412901/1169123322538233886/Cricket-01-01.png?ex=655441f1&amp;is=6541ccf1&amp;hm=58f97afb651174ae4f7a6061aec121c2e63fc7aba60ba61763f84a721f630bf2&amp;=&amp;width=606&amp;height=662</t>
@@ -463,7 +460,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -489,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -516,13 +513,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -546,13 +543,13 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -576,19 +573,19 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
         <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -714,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J8" s="1"/>
     </row>

</xml_diff>